<commit_message>
NEED TO TEST THE MRINV CASES
</commit_message>
<xml_diff>
--- a/NewVersionmay2017/A_R calculation.xlsx
+++ b/NewVersionmay2017/A_R calculation.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="11970" windowHeight="7365" firstSheet="5" activeTab="10"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="11970" windowHeight="7365" firstSheet="5" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="p is 124" sheetId="1" r:id="rId1"/>
@@ -18,11 +18,13 @@
     <sheet name="p is 134" sheetId="2" r:id="rId4"/>
     <sheet name="different p 124" sheetId="5" r:id="rId5"/>
     <sheet name="upper triangular mi5" sheetId="6" r:id="rId6"/>
-    <sheet name="2 pivot mi5 example" sheetId="8" r:id="rId7"/>
-    <sheet name="Sheet5" sheetId="7" r:id="rId8"/>
-    <sheet name="Sheet4" sheetId="10" r:id="rId9"/>
-    <sheet name="basis" sheetId="9" r:id="rId10"/>
-    <sheet name="linearly dependent problem" sheetId="11" r:id="rId11"/>
+    <sheet name="Sheet6" sheetId="13" r:id="rId7"/>
+    <sheet name="Sheet3" sheetId="12" r:id="rId8"/>
+    <sheet name="2 pivot mi5 example" sheetId="8" r:id="rId9"/>
+    <sheet name="Sheet5" sheetId="7" r:id="rId10"/>
+    <sheet name="Sheet4" sheetId="10" r:id="rId11"/>
+    <sheet name="basis" sheetId="9" r:id="rId12"/>
+    <sheet name="linearly dependent problem" sheetId="11" r:id="rId13"/>
   </sheets>
   <calcPr calcId="171027" calcOnSave="0" concurrentCalc="0"/>
   <extLst>
@@ -34,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="80">
   <si>
     <t>V</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -299,6 +301,14 @@
   </si>
   <si>
     <t xml:space="preserve"> ((2 3) -)</t>
+  </si>
+  <si>
+    <t>E_X</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>EX</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -1340,6 +1350,731 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:M14"/>
+  <sheetViews>
+    <sheetView zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
+      <selection activeCell="O15" sqref="O15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="8" width="3.5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="3.5" customWidth="1"/>
+    <col min="10" max="14" width="4.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B1">
+        <v>35</v>
+      </c>
+      <c r="C1">
+        <v>14</v>
+      </c>
+      <c r="D1">
+        <v>24</v>
+      </c>
+      <c r="E1">
+        <v>15</v>
+      </c>
+      <c r="F1">
+        <v>34</v>
+      </c>
+      <c r="G1">
+        <v>25</v>
+      </c>
+      <c r="H1">
+        <v>13</v>
+      </c>
+      <c r="I1">
+        <v>45</v>
+      </c>
+      <c r="J1">
+        <v>125</v>
+      </c>
+      <c r="K1">
+        <v>234</v>
+      </c>
+      <c r="L1">
+        <v>124</v>
+      </c>
+      <c r="M1">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A2" s="6">
+        <v>4</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1"/>
+      <c r="J2" s="1"/>
+      <c r="K2" s="1">
+        <v>-1</v>
+      </c>
+      <c r="L2" s="1">
+        <v>-1</v>
+      </c>
+      <c r="M2" s="1"/>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A3" s="6">
+        <v>5</v>
+      </c>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
+      <c r="I3" s="1"/>
+      <c r="J3" s="1">
+        <v>-1</v>
+      </c>
+      <c r="K3" s="1"/>
+      <c r="L3" s="1"/>
+      <c r="M3" s="1">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>35</v>
+      </c>
+      <c r="B4" s="1">
+        <v>1</v>
+      </c>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1"/>
+      <c r="I4" s="1"/>
+      <c r="J4" s="1"/>
+      <c r="K4" s="1"/>
+      <c r="L4" s="1"/>
+      <c r="M4" s="1">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>14</v>
+      </c>
+      <c r="B5" s="1"/>
+      <c r="C5" s="1">
+        <v>1</v>
+      </c>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1"/>
+      <c r="I5" s="1"/>
+      <c r="J5" s="1"/>
+      <c r="K5" s="1"/>
+      <c r="L5" s="1">
+        <v>-1</v>
+      </c>
+      <c r="M5" s="1"/>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>24</v>
+      </c>
+      <c r="B6" s="1"/>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1">
+        <v>1</v>
+      </c>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1"/>
+      <c r="I6" s="1"/>
+      <c r="J6" s="1"/>
+      <c r="K6" s="1">
+        <v>-1</v>
+      </c>
+      <c r="L6" s="1">
+        <v>-1</v>
+      </c>
+      <c r="M6" s="1"/>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>15</v>
+      </c>
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1">
+        <v>1</v>
+      </c>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1"/>
+      <c r="H7" s="1"/>
+      <c r="I7" s="1"/>
+      <c r="J7" s="1">
+        <v>-1</v>
+      </c>
+      <c r="K7" s="1"/>
+      <c r="L7" s="1"/>
+      <c r="M7" s="1">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>34</v>
+      </c>
+      <c r="B8" s="1"/>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1">
+        <v>1</v>
+      </c>
+      <c r="G8" s="1"/>
+      <c r="H8" s="1"/>
+      <c r="I8" s="1"/>
+      <c r="J8" s="1"/>
+      <c r="K8" s="1">
+        <v>-1</v>
+      </c>
+      <c r="L8" s="1"/>
+      <c r="M8" s="1"/>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>25</v>
+      </c>
+      <c r="B9" s="1"/>
+      <c r="C9" s="1"/>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1"/>
+      <c r="F9" s="1"/>
+      <c r="G9" s="1">
+        <v>1</v>
+      </c>
+      <c r="H9" s="1"/>
+      <c r="I9" s="1"/>
+      <c r="J9" s="1">
+        <v>-1</v>
+      </c>
+      <c r="K9" s="1"/>
+      <c r="L9" s="1"/>
+      <c r="M9" s="1"/>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>13</v>
+      </c>
+      <c r="B10" s="1"/>
+      <c r="C10" s="1"/>
+      <c r="D10" s="1"/>
+      <c r="E10" s="1"/>
+      <c r="F10" s="1"/>
+      <c r="G10" s="1"/>
+      <c r="H10" s="1">
+        <v>1</v>
+      </c>
+      <c r="I10" s="1"/>
+      <c r="J10" s="1"/>
+      <c r="K10" s="1"/>
+      <c r="L10" s="1"/>
+      <c r="M10" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>45</v>
+      </c>
+      <c r="B11" s="1"/>
+      <c r="C11" s="1"/>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1"/>
+      <c r="F11" s="1"/>
+      <c r="G11" s="1"/>
+      <c r="H11" s="1"/>
+      <c r="I11" s="1">
+        <v>1</v>
+      </c>
+      <c r="J11" s="1"/>
+      <c r="K11" s="1"/>
+      <c r="L11" s="1"/>
+      <c r="M11" s="1"/>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A12" s="7">
+        <v>12</v>
+      </c>
+      <c r="B12" s="1"/>
+      <c r="C12" s="1"/>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1"/>
+      <c r="G12" s="1"/>
+      <c r="H12" s="1"/>
+      <c r="I12" s="1"/>
+      <c r="J12" s="1">
+        <v>1</v>
+      </c>
+      <c r="K12" s="1"/>
+      <c r="L12" s="1">
+        <v>1</v>
+      </c>
+      <c r="M12" s="1"/>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A13" s="6">
+        <v>23</v>
+      </c>
+      <c r="B13" s="1"/>
+      <c r="C13" s="1"/>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1"/>
+      <c r="F13" s="1"/>
+      <c r="G13" s="1"/>
+      <c r="H13" s="1"/>
+      <c r="I13" s="1"/>
+      <c r="J13" s="1"/>
+      <c r="K13" s="1">
+        <v>1</v>
+      </c>
+      <c r="L13" s="1"/>
+      <c r="M13" s="1"/>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="K14" s="5"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G27"/>
+  <sheetViews>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="J32" sqref="J32"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1">
+        <v>4</v>
+      </c>
+      <c r="C1">
+        <v>4</v>
+      </c>
+      <c r="E1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>5</v>
+      </c>
+      <c r="C2">
+        <v>5</v>
+      </c>
+      <c r="E2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B3" t="s">
+        <v>32</v>
+      </c>
+      <c r="C3" t="str">
+        <f>_xlfn.CONCAT(A3,B3)</f>
+        <v xml:space="preserve"> (1 2)</v>
+      </c>
+      <c r="E3" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>31</v>
+      </c>
+      <c r="B4" t="s">
+        <v>33</v>
+      </c>
+      <c r="C4" t="str">
+        <f t="shared" ref="C4:C12" si="0">_xlfn.CONCAT(A4,B4)</f>
+        <v xml:space="preserve"> (1 3)</v>
+      </c>
+      <c r="E4" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>34</v>
+      </c>
+      <c r="B5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C5" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> (2 3)</v>
+      </c>
+      <c r="E5" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>31</v>
+      </c>
+      <c r="B6" t="s">
+        <v>35</v>
+      </c>
+      <c r="C6" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> (1 4)</v>
+      </c>
+      <c r="E6" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>34</v>
+      </c>
+      <c r="B7" t="s">
+        <v>35</v>
+      </c>
+      <c r="C7" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> (2 4)</v>
+      </c>
+      <c r="E7" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>36</v>
+      </c>
+      <c r="B8" t="s">
+        <v>35</v>
+      </c>
+      <c r="C8" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> (3 4)</v>
+      </c>
+      <c r="E8" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>31</v>
+      </c>
+      <c r="B9" t="s">
+        <v>37</v>
+      </c>
+      <c r="C9" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> (1 5)</v>
+      </c>
+      <c r="E9" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>34</v>
+      </c>
+      <c r="B10" t="s">
+        <v>37</v>
+      </c>
+      <c r="C10" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> (2 5)</v>
+      </c>
+      <c r="E10" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>36</v>
+      </c>
+      <c r="B11" t="s">
+        <v>37</v>
+      </c>
+      <c r="C11" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> (3 5)</v>
+      </c>
+      <c r="E11" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>38</v>
+      </c>
+      <c r="B12" t="s">
+        <v>37</v>
+      </c>
+      <c r="C12" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve"> (4 5)</v>
+      </c>
+      <c r="E12" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>49</v>
+      </c>
+      <c r="B16" t="s">
+        <v>37</v>
+      </c>
+      <c r="C16" t="s">
+        <v>50</v>
+      </c>
+      <c r="E16" t="str">
+        <f>_xlfn.CONCAT(A16,B16,C16)</f>
+        <v>((3 5) None)</v>
+      </c>
+      <c r="G16" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>51</v>
+      </c>
+      <c r="B17" t="s">
+        <v>35</v>
+      </c>
+      <c r="C17" t="s">
+        <v>50</v>
+      </c>
+      <c r="E17" t="str">
+        <f t="shared" ref="E17:E27" si="1">_xlfn.CONCAT(A17,B17,C17)</f>
+        <v xml:space="preserve"> ((2 4) None)</v>
+      </c>
+      <c r="G17" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>52</v>
+      </c>
+      <c r="B18" t="s">
+        <v>35</v>
+      </c>
+      <c r="C18" t="s">
+        <v>37</v>
+      </c>
+      <c r="E18" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve"> ((1 4) 5)</v>
+      </c>
+      <c r="G18" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>52</v>
+      </c>
+      <c r="B19" t="s">
+        <v>37</v>
+      </c>
+      <c r="C19" t="s">
+        <v>50</v>
+      </c>
+      <c r="E19" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve"> ((1 5) None)</v>
+      </c>
+      <c r="G19" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>53</v>
+      </c>
+      <c r="B20" t="s">
+        <v>35</v>
+      </c>
+      <c r="C20" t="s">
+        <v>50</v>
+      </c>
+      <c r="E20" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve"> ((3 4) None)</v>
+      </c>
+      <c r="G20" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>51</v>
+      </c>
+      <c r="B21" t="s">
+        <v>37</v>
+      </c>
+      <c r="C21" t="s">
+        <v>50</v>
+      </c>
+      <c r="E21" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve"> ((2 5) None)</v>
+      </c>
+      <c r="G21" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>52</v>
+      </c>
+      <c r="B22" t="s">
+        <v>33</v>
+      </c>
+      <c r="C22" t="s">
+        <v>50</v>
+      </c>
+      <c r="E22" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve"> ((1 3) None)</v>
+      </c>
+      <c r="G22" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>54</v>
+      </c>
+      <c r="B23" t="s">
+        <v>37</v>
+      </c>
+      <c r="C23" t="s">
+        <v>50</v>
+      </c>
+      <c r="E23" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve"> ((4 5) None)</v>
+      </c>
+      <c r="G23" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>51</v>
+      </c>
+      <c r="B24" t="s">
+        <v>33</v>
+      </c>
+      <c r="C24" t="s">
+        <v>35</v>
+      </c>
+      <c r="E24" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve"> ((2 3) 4)</v>
+      </c>
+      <c r="G24" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>52</v>
+      </c>
+      <c r="B25" t="s">
+        <v>32</v>
+      </c>
+      <c r="C25" t="s">
+        <v>50</v>
+      </c>
+      <c r="E25" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve"> ((1 2) None)</v>
+      </c>
+      <c r="G25" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>52</v>
+      </c>
+      <c r="B26" t="s">
+        <v>33</v>
+      </c>
+      <c r="C26" t="s">
+        <v>35</v>
+      </c>
+      <c r="E26" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve"> ((1 3) 4)</v>
+      </c>
+      <c r="G26" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>52</v>
+      </c>
+      <c r="B27" t="s">
+        <v>33</v>
+      </c>
+      <c r="C27" t="s">
+        <v>37</v>
+      </c>
+      <c r="E27" t="str">
+        <f t="shared" si="1"/>
+        <v xml:space="preserve"> ((1 3) 5)</v>
+      </c>
+      <c r="G27" t="s">
+        <v>66</v>
+      </c>
+    </row>
+  </sheetData>
+  <dataConsolidate/>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M32"/>
   <sheetViews>
     <sheetView topLeftCell="A10" workbookViewId="0">
@@ -2108,11 +2843,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
@@ -3410,7 +4145,7 @@
   <dimension ref="A1:U15"/>
   <sheetViews>
     <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="J18" sqref="J18"/>
+      <selection activeCell="B1" sqref="B1:N14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -3853,6 +4588,1461 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:N14"/>
+  <sheetViews>
+    <sheetView zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="J2" sqref="J2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="9" width="3.5" bestFit="1" customWidth="1"/>
+    <col min="10" max="13" width="4.5" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="3.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="B1" t="s">
+        <v>22</v>
+      </c>
+      <c r="L1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B2">
+        <v>35</v>
+      </c>
+      <c r="C2">
+        <v>45</v>
+      </c>
+      <c r="D2">
+        <v>12</v>
+      </c>
+      <c r="E2">
+        <v>24</v>
+      </c>
+      <c r="F2">
+        <v>25</v>
+      </c>
+      <c r="G2">
+        <v>13</v>
+      </c>
+      <c r="H2">
+        <v>14</v>
+      </c>
+      <c r="I2">
+        <v>15</v>
+      </c>
+      <c r="J2">
+        <v>345</v>
+      </c>
+      <c r="K2">
+        <v>234</v>
+      </c>
+      <c r="L2">
+        <v>145</v>
+      </c>
+      <c r="M2">
+        <v>234</v>
+      </c>
+      <c r="N2">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A3" s="6">
+        <v>4</v>
+      </c>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
+      <c r="I3" s="1"/>
+      <c r="J3" s="1"/>
+      <c r="K3" s="1">
+        <v>-1</v>
+      </c>
+      <c r="L3" s="1"/>
+      <c r="M3" s="1">
+        <v>-1</v>
+      </c>
+      <c r="N3">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A4" s="6">
+        <v>5</v>
+      </c>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1"/>
+      <c r="I4" s="1"/>
+      <c r="J4" s="1">
+        <v>-1</v>
+      </c>
+      <c r="K4" s="1"/>
+      <c r="L4" s="1">
+        <v>-1</v>
+      </c>
+      <c r="M4" s="1"/>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A5" s="7">
+        <v>35</v>
+      </c>
+      <c r="B5" s="1">
+        <v>1</v>
+      </c>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1"/>
+      <c r="I5" s="1"/>
+      <c r="J5" s="1"/>
+      <c r="K5" s="1"/>
+      <c r="L5" s="1"/>
+      <c r="M5" s="1"/>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A6" s="7">
+        <v>45</v>
+      </c>
+      <c r="B6" s="1"/>
+      <c r="C6" s="1">
+        <v>1</v>
+      </c>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1"/>
+      <c r="I6" s="1"/>
+      <c r="J6" s="1"/>
+      <c r="K6" s="1"/>
+      <c r="L6" s="1">
+        <v>-1</v>
+      </c>
+      <c r="M6" s="1"/>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A7" s="7">
+        <v>12</v>
+      </c>
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1">
+        <v>1</v>
+      </c>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1"/>
+      <c r="H7" s="1"/>
+      <c r="I7" s="1"/>
+      <c r="J7" s="1"/>
+      <c r="K7" s="1"/>
+      <c r="L7" s="1"/>
+      <c r="M7" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A8" s="7">
+        <v>24</v>
+      </c>
+      <c r="B8" s="1"/>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1">
+        <v>1</v>
+      </c>
+      <c r="F8" s="1"/>
+      <c r="G8" s="1"/>
+      <c r="H8" s="1"/>
+      <c r="I8" s="1"/>
+      <c r="J8" s="1">
+        <v>-1</v>
+      </c>
+      <c r="K8" s="1"/>
+      <c r="L8" s="1"/>
+      <c r="M8" s="1">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A9" s="7">
+        <v>25</v>
+      </c>
+      <c r="B9" s="1"/>
+      <c r="C9" s="1"/>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1"/>
+      <c r="F9" s="1">
+        <v>1</v>
+      </c>
+      <c r="G9" s="1"/>
+      <c r="H9" s="1"/>
+      <c r="I9" s="1"/>
+      <c r="J9" s="1"/>
+      <c r="K9" s="1"/>
+      <c r="L9" s="1"/>
+      <c r="M9" s="1"/>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A10" s="7">
+        <v>13</v>
+      </c>
+      <c r="B10" s="1"/>
+      <c r="C10" s="1"/>
+      <c r="D10" s="1"/>
+      <c r="E10" s="1"/>
+      <c r="F10" s="1"/>
+      <c r="G10" s="1">
+        <v>1</v>
+      </c>
+      <c r="H10" s="1"/>
+      <c r="I10" s="1"/>
+      <c r="J10" s="1"/>
+      <c r="K10" s="1"/>
+      <c r="L10" s="1"/>
+      <c r="M10" s="1">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A11" s="7">
+        <v>14</v>
+      </c>
+      <c r="B11" s="1"/>
+      <c r="C11" s="1"/>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1"/>
+      <c r="F11" s="1"/>
+      <c r="G11" s="1"/>
+      <c r="H11" s="1">
+        <v>1</v>
+      </c>
+      <c r="I11" s="1"/>
+      <c r="J11" s="1"/>
+      <c r="K11" s="1"/>
+      <c r="L11" s="1">
+        <v>1</v>
+      </c>
+      <c r="M11" s="1"/>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A12" s="7">
+        <v>15</v>
+      </c>
+      <c r="B12" s="1"/>
+      <c r="C12" s="1"/>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1"/>
+      <c r="G12" s="1"/>
+      <c r="H12" s="1"/>
+      <c r="I12" s="1">
+        <v>1</v>
+      </c>
+      <c r="J12" s="1"/>
+      <c r="K12" s="1"/>
+      <c r="L12" s="1">
+        <v>-1</v>
+      </c>
+      <c r="M12" s="1"/>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A13" s="6">
+        <v>34</v>
+      </c>
+      <c r="B13" s="1"/>
+      <c r="C13" s="1"/>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1"/>
+      <c r="F13" s="1"/>
+      <c r="G13" s="1"/>
+      <c r="H13" s="1"/>
+      <c r="I13" s="1"/>
+      <c r="J13" s="1">
+        <v>1</v>
+      </c>
+      <c r="K13" s="1"/>
+      <c r="L13" s="1"/>
+      <c r="M13" s="1"/>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A14" s="6">
+        <v>23</v>
+      </c>
+      <c r="B14" s="1"/>
+      <c r="C14" s="1"/>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
+      <c r="F14" s="1"/>
+      <c r="G14" s="1"/>
+      <c r="H14" s="1"/>
+      <c r="I14" s="1"/>
+      <c r="J14" s="1"/>
+      <c r="K14" s="1">
+        <v>1</v>
+      </c>
+      <c r="L14" s="1"/>
+      <c r="M14" s="1"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:N66"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A52" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="G56" sqref="G56"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="4.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="5" width="3.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="4.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="3.5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="4.5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="4" customWidth="1"/>
+    <col min="10" max="13" width="4.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B1" t="s">
+        <v>22</v>
+      </c>
+      <c r="L1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B2">
+        <v>35</v>
+      </c>
+      <c r="C2">
+        <v>45</v>
+      </c>
+      <c r="D2">
+        <v>23</v>
+      </c>
+      <c r="E2">
+        <v>24</v>
+      </c>
+      <c r="F2">
+        <v>25</v>
+      </c>
+      <c r="G2">
+        <v>34</v>
+      </c>
+      <c r="H2">
+        <v>15</v>
+      </c>
+      <c r="I2">
+        <v>14</v>
+      </c>
+      <c r="J2">
+        <v>125</v>
+      </c>
+      <c r="K2">
+        <v>134</v>
+      </c>
+      <c r="L2">
+        <v>234</v>
+      </c>
+      <c r="M2">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A3" s="6">
+        <v>4</v>
+      </c>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
+      <c r="I3" s="1"/>
+      <c r="J3" s="1"/>
+      <c r="K3" s="1">
+        <v>-1</v>
+      </c>
+      <c r="L3" s="1">
+        <v>-1</v>
+      </c>
+      <c r="M3" s="1"/>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A4" s="6">
+        <v>5</v>
+      </c>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1"/>
+      <c r="I4" s="1"/>
+      <c r="J4" s="1">
+        <v>-1</v>
+      </c>
+      <c r="K4" s="1"/>
+      <c r="L4" s="1"/>
+      <c r="M4" s="1">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A5" s="7">
+        <v>35</v>
+      </c>
+      <c r="B5" s="1">
+        <v>1</v>
+      </c>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1"/>
+      <c r="I5" s="1"/>
+      <c r="J5" s="1"/>
+      <c r="K5" s="1"/>
+      <c r="L5" s="1"/>
+      <c r="M5" s="1"/>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A6" s="7">
+        <v>45</v>
+      </c>
+      <c r="B6" s="1"/>
+      <c r="C6" s="1">
+        <v>1</v>
+      </c>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1"/>
+      <c r="I6" s="1"/>
+      <c r="J6" s="1"/>
+      <c r="K6" s="1"/>
+      <c r="L6" s="1"/>
+      <c r="M6" s="1">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A7" s="7">
+        <v>23</v>
+      </c>
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1">
+        <v>1</v>
+      </c>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1"/>
+      <c r="H7" s="1"/>
+      <c r="I7" s="1"/>
+      <c r="J7" s="1"/>
+      <c r="K7" s="1"/>
+      <c r="L7" s="1">
+        <v>1</v>
+      </c>
+      <c r="M7" s="1"/>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A8" s="7">
+        <v>24</v>
+      </c>
+      <c r="B8" s="1"/>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1">
+        <v>1</v>
+      </c>
+      <c r="F8" s="1"/>
+      <c r="G8" s="1"/>
+      <c r="H8" s="1"/>
+      <c r="I8" s="1"/>
+      <c r="J8" s="1"/>
+      <c r="K8" s="1"/>
+      <c r="L8" s="1">
+        <v>-1</v>
+      </c>
+      <c r="M8" s="1"/>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A9" s="7">
+        <v>25</v>
+      </c>
+      <c r="B9" s="1"/>
+      <c r="C9" s="1"/>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1"/>
+      <c r="F9" s="1">
+        <v>1</v>
+      </c>
+      <c r="G9" s="1"/>
+      <c r="H9" s="1"/>
+      <c r="I9" s="1"/>
+      <c r="J9" s="1">
+        <v>-1</v>
+      </c>
+      <c r="K9" s="1"/>
+      <c r="L9" s="1"/>
+      <c r="M9" s="1"/>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A10" s="7">
+        <v>34</v>
+      </c>
+      <c r="B10" s="1"/>
+      <c r="C10" s="1"/>
+      <c r="D10" s="1"/>
+      <c r="E10" s="1"/>
+      <c r="F10" s="1"/>
+      <c r="G10" s="1">
+        <v>1</v>
+      </c>
+      <c r="H10" s="1"/>
+      <c r="I10" s="1"/>
+      <c r="J10" s="1"/>
+      <c r="K10" s="1">
+        <v>-1</v>
+      </c>
+      <c r="L10" s="1">
+        <v>-1</v>
+      </c>
+      <c r="M10" s="1"/>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A11" s="7">
+        <v>15</v>
+      </c>
+      <c r="B11" s="1"/>
+      <c r="C11" s="1"/>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1"/>
+      <c r="F11" s="1"/>
+      <c r="G11" s="1"/>
+      <c r="H11" s="1">
+        <v>1</v>
+      </c>
+      <c r="J11" s="1">
+        <v>-1</v>
+      </c>
+      <c r="L11" s="1"/>
+      <c r="M11" s="1">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A12" s="7">
+        <v>14</v>
+      </c>
+      <c r="B12" s="1"/>
+      <c r="C12" s="1"/>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1"/>
+      <c r="G12" s="1"/>
+      <c r="I12" s="1">
+        <v>1</v>
+      </c>
+      <c r="K12" s="1">
+        <v>-1</v>
+      </c>
+      <c r="L12" s="1"/>
+      <c r="M12" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A13" s="6">
+        <v>12</v>
+      </c>
+      <c r="B13" s="1"/>
+      <c r="C13" s="1"/>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1"/>
+      <c r="F13" s="1"/>
+      <c r="G13" s="1"/>
+      <c r="H13" s="1"/>
+      <c r="I13" s="1"/>
+      <c r="J13" s="1">
+        <v>1</v>
+      </c>
+      <c r="K13" s="1"/>
+      <c r="L13" s="1"/>
+      <c r="M13" s="1"/>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A14" s="6">
+        <v>13</v>
+      </c>
+      <c r="B14" s="1"/>
+      <c r="C14" s="1"/>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
+      <c r="F14" s="1"/>
+      <c r="G14" s="1"/>
+      <c r="H14" s="1"/>
+      <c r="I14" s="1"/>
+      <c r="J14" s="1"/>
+      <c r="K14" s="1">
+        <v>1</v>
+      </c>
+      <c r="L14" s="1"/>
+      <c r="M14" s="1"/>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B17" t="s">
+        <v>22</v>
+      </c>
+      <c r="L17" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>26</v>
+      </c>
+      <c r="B18">
+        <v>35</v>
+      </c>
+      <c r="C18">
+        <v>45</v>
+      </c>
+      <c r="D18">
+        <v>23</v>
+      </c>
+      <c r="E18">
+        <v>24</v>
+      </c>
+      <c r="F18">
+        <v>25</v>
+      </c>
+      <c r="G18">
+        <v>34</v>
+      </c>
+      <c r="H18">
+        <v>15</v>
+      </c>
+      <c r="I18">
+        <v>145</v>
+      </c>
+      <c r="J18">
+        <v>125</v>
+      </c>
+      <c r="K18">
+        <v>134</v>
+      </c>
+      <c r="L18">
+        <v>234</v>
+      </c>
+      <c r="M18">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A19" s="6">
+        <v>4</v>
+      </c>
+      <c r="B19" s="1"/>
+      <c r="C19" s="1"/>
+      <c r="D19" s="1"/>
+      <c r="E19" s="1"/>
+      <c r="F19" s="1"/>
+      <c r="G19" s="1"/>
+      <c r="H19" s="1"/>
+      <c r="I19" s="1"/>
+      <c r="J19" s="1"/>
+      <c r="K19" s="1">
+        <v>-1</v>
+      </c>
+      <c r="L19" s="1">
+        <v>-1</v>
+      </c>
+      <c r="M19" s="1"/>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A20" s="6">
+        <v>5</v>
+      </c>
+      <c r="B20" s="1"/>
+      <c r="C20" s="1"/>
+      <c r="D20" s="1"/>
+      <c r="E20" s="1"/>
+      <c r="F20" s="1"/>
+      <c r="G20" s="1"/>
+      <c r="H20" s="1"/>
+      <c r="I20" s="1">
+        <v>-1</v>
+      </c>
+      <c r="J20" s="1">
+        <v>-1</v>
+      </c>
+      <c r="K20" s="1"/>
+      <c r="L20" s="1"/>
+      <c r="M20" s="1"/>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A21" s="7">
+        <v>35</v>
+      </c>
+      <c r="B21" s="1">
+        <v>1</v>
+      </c>
+      <c r="C21" s="1"/>
+      <c r="D21" s="1"/>
+      <c r="E21" s="1"/>
+      <c r="F21" s="1"/>
+      <c r="G21" s="1"/>
+      <c r="H21" s="1"/>
+      <c r="I21" s="1"/>
+      <c r="J21" s="1"/>
+      <c r="K21" s="1"/>
+      <c r="L21" s="1"/>
+      <c r="M21" s="1"/>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A22" s="7">
+        <v>45</v>
+      </c>
+      <c r="B22" s="1"/>
+      <c r="C22" s="1">
+        <v>1</v>
+      </c>
+      <c r="D22" s="1"/>
+      <c r="E22" s="1"/>
+      <c r="F22" s="1"/>
+      <c r="G22" s="1"/>
+      <c r="H22" s="1"/>
+      <c r="I22" s="1">
+        <v>-1</v>
+      </c>
+      <c r="J22" s="1"/>
+      <c r="K22" s="1"/>
+      <c r="L22" s="1"/>
+      <c r="M22" s="1"/>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A23" s="7">
+        <v>23</v>
+      </c>
+      <c r="B23" s="1"/>
+      <c r="C23" s="1"/>
+      <c r="D23" s="1">
+        <v>1</v>
+      </c>
+      <c r="E23" s="1"/>
+      <c r="F23" s="1"/>
+      <c r="G23" s="1"/>
+      <c r="H23" s="1"/>
+      <c r="I23" s="1"/>
+      <c r="J23" s="1"/>
+      <c r="K23" s="1"/>
+      <c r="L23" s="1">
+        <v>1</v>
+      </c>
+      <c r="M23" s="1"/>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A24" s="7">
+        <v>24</v>
+      </c>
+      <c r="B24" s="1"/>
+      <c r="C24" s="1"/>
+      <c r="D24" s="1"/>
+      <c r="E24" s="1">
+        <v>1</v>
+      </c>
+      <c r="F24" s="1"/>
+      <c r="G24" s="1"/>
+      <c r="H24" s="1"/>
+      <c r="I24" s="1"/>
+      <c r="J24" s="1"/>
+      <c r="K24" s="1"/>
+      <c r="L24" s="1">
+        <v>-1</v>
+      </c>
+      <c r="M24" s="1"/>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A25" s="7">
+        <v>25</v>
+      </c>
+      <c r="B25" s="1"/>
+      <c r="C25" s="1"/>
+      <c r="D25" s="1"/>
+      <c r="E25" s="1"/>
+      <c r="F25" s="1">
+        <v>1</v>
+      </c>
+      <c r="G25" s="1"/>
+      <c r="H25" s="1"/>
+      <c r="I25" s="1"/>
+      <c r="J25" s="1">
+        <v>-1</v>
+      </c>
+      <c r="K25" s="1"/>
+      <c r="L25" s="1"/>
+      <c r="M25" s="1"/>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A26" s="7">
+        <v>34</v>
+      </c>
+      <c r="B26" s="1"/>
+      <c r="C26" s="1"/>
+      <c r="D26" s="1"/>
+      <c r="E26" s="1"/>
+      <c r="F26" s="1"/>
+      <c r="G26" s="1">
+        <v>1</v>
+      </c>
+      <c r="H26" s="1"/>
+      <c r="I26" s="1"/>
+      <c r="J26" s="1"/>
+      <c r="K26" s="1">
+        <v>-1</v>
+      </c>
+      <c r="L26" s="1">
+        <v>-1</v>
+      </c>
+      <c r="M26" s="1"/>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A27" s="7">
+        <v>15</v>
+      </c>
+      <c r="B27" s="1"/>
+      <c r="C27" s="1"/>
+      <c r="D27" s="1"/>
+      <c r="E27" s="1"/>
+      <c r="F27" s="1"/>
+      <c r="G27" s="1"/>
+      <c r="H27" s="1">
+        <v>1</v>
+      </c>
+      <c r="I27" s="1">
+        <v>-1</v>
+      </c>
+      <c r="J27" s="1">
+        <v>-1</v>
+      </c>
+      <c r="L27" s="1"/>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A28" s="7">
+        <v>14</v>
+      </c>
+      <c r="B28" s="1"/>
+      <c r="C28" s="1"/>
+      <c r="D28" s="1"/>
+      <c r="E28" s="1"/>
+      <c r="F28" s="1"/>
+      <c r="G28" s="1"/>
+      <c r="I28" s="1">
+        <v>1</v>
+      </c>
+      <c r="K28" s="1">
+        <v>-1</v>
+      </c>
+      <c r="L28" s="1"/>
+      <c r="M28" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A29" s="6">
+        <v>12</v>
+      </c>
+      <c r="B29" s="1"/>
+      <c r="C29" s="1"/>
+      <c r="D29" s="1"/>
+      <c r="E29" s="1"/>
+      <c r="F29" s="1"/>
+      <c r="G29" s="1"/>
+      <c r="H29" s="1"/>
+      <c r="I29" s="1"/>
+      <c r="J29" s="1">
+        <v>1</v>
+      </c>
+      <c r="K29" s="1"/>
+      <c r="L29" s="1"/>
+      <c r="M29" s="1"/>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A30" s="6">
+        <v>13</v>
+      </c>
+      <c r="B30" s="1"/>
+      <c r="C30" s="1"/>
+      <c r="D30" s="1"/>
+      <c r="E30" s="1"/>
+      <c r="F30" s="1"/>
+      <c r="G30" s="1"/>
+      <c r="H30" s="1"/>
+      <c r="I30" s="1"/>
+      <c r="J30" s="1"/>
+      <c r="K30" s="1">
+        <v>1</v>
+      </c>
+      <c r="L30" s="1"/>
+      <c r="M30" s="1"/>
+    </row>
+    <row r="34" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B34" t="s">
+        <v>22</v>
+      </c>
+      <c r="J34" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>26</v>
+      </c>
+      <c r="B35">
+        <v>24</v>
+      </c>
+      <c r="C35">
+        <v>15</v>
+      </c>
+      <c r="D35">
+        <v>34</v>
+      </c>
+      <c r="E35">
+        <v>23</v>
+      </c>
+      <c r="F35">
+        <v>25</v>
+      </c>
+      <c r="G35">
+        <v>45</v>
+      </c>
+      <c r="H35">
+        <v>134</v>
+      </c>
+      <c r="I35">
+        <v>125</v>
+      </c>
+      <c r="J35">
+        <v>234</v>
+      </c>
+      <c r="K35">
+        <v>145</v>
+      </c>
+      <c r="L35">
+        <v>120</v>
+      </c>
+      <c r="M35">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A36" s="6">
+        <v>4</v>
+      </c>
+      <c r="B36" s="1"/>
+      <c r="C36" s="1"/>
+      <c r="D36" s="1"/>
+      <c r="E36" s="1"/>
+      <c r="F36" s="1"/>
+      <c r="G36" s="1"/>
+      <c r="H36" s="1"/>
+      <c r="I36" s="1"/>
+      <c r="J36" s="1"/>
+      <c r="K36" s="1"/>
+      <c r="L36" s="1"/>
+      <c r="M36" s="1"/>
+    </row>
+    <row r="37" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A37" s="6">
+        <v>5</v>
+      </c>
+      <c r="B37" s="1"/>
+      <c r="C37" s="1"/>
+      <c r="D37" s="1"/>
+      <c r="E37" s="1"/>
+      <c r="F37" s="1"/>
+      <c r="G37" s="1"/>
+      <c r="H37" s="1"/>
+      <c r="I37" s="1"/>
+      <c r="J37" s="1"/>
+      <c r="K37" s="1"/>
+      <c r="L37" s="1"/>
+      <c r="M37" s="1"/>
+    </row>
+    <row r="38" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A38" s="7">
+        <v>14</v>
+      </c>
+      <c r="B38" s="1"/>
+      <c r="C38" s="1"/>
+      <c r="D38" s="1"/>
+      <c r="E38" s="1"/>
+      <c r="F38" s="1"/>
+      <c r="G38" s="1"/>
+      <c r="H38" s="1"/>
+      <c r="I38" s="1"/>
+      <c r="J38" s="1"/>
+      <c r="K38" s="1"/>
+      <c r="L38" s="1"/>
+      <c r="M38" s="1"/>
+    </row>
+    <row r="39" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A39" s="7">
+        <v>35</v>
+      </c>
+      <c r="B39" s="1"/>
+      <c r="C39" s="1"/>
+      <c r="D39" s="1"/>
+      <c r="E39" s="1"/>
+      <c r="F39" s="1"/>
+      <c r="G39" s="1"/>
+      <c r="H39" s="1"/>
+      <c r="I39" s="1"/>
+      <c r="J39" s="1"/>
+      <c r="K39" s="1"/>
+      <c r="L39" s="1"/>
+      <c r="M39" s="1"/>
+    </row>
+    <row r="40" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A40">
+        <v>24</v>
+      </c>
+      <c r="B40" s="1">
+        <v>1</v>
+      </c>
+      <c r="C40" s="1"/>
+      <c r="D40" s="1"/>
+      <c r="E40" s="1"/>
+      <c r="F40" s="1"/>
+      <c r="G40" s="1"/>
+      <c r="H40" s="1"/>
+      <c r="I40" s="1"/>
+      <c r="J40" s="1"/>
+      <c r="K40" s="1"/>
+      <c r="L40" s="1"/>
+      <c r="M40" s="1"/>
+    </row>
+    <row r="41" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A41">
+        <v>15</v>
+      </c>
+      <c r="B41" s="1"/>
+      <c r="C41" s="1">
+        <v>1</v>
+      </c>
+      <c r="D41" s="1"/>
+      <c r="E41" s="1"/>
+      <c r="F41" s="1"/>
+      <c r="G41" s="1"/>
+      <c r="H41" s="1"/>
+      <c r="I41" s="1"/>
+      <c r="J41" s="1"/>
+      <c r="K41" s="1"/>
+      <c r="L41" s="1"/>
+      <c r="M41" s="1"/>
+    </row>
+    <row r="42" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A42">
+        <v>34</v>
+      </c>
+      <c r="B42" s="1"/>
+      <c r="C42" s="1"/>
+      <c r="D42" s="1">
+        <v>1</v>
+      </c>
+      <c r="E42" s="1"/>
+      <c r="F42" s="1"/>
+      <c r="G42" s="1"/>
+      <c r="H42" s="1"/>
+      <c r="I42" s="1"/>
+      <c r="J42" s="1"/>
+      <c r="K42" s="1"/>
+      <c r="L42" s="1"/>
+      <c r="M42" s="1"/>
+    </row>
+    <row r="43" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A43">
+        <v>23</v>
+      </c>
+      <c r="B43" s="1"/>
+      <c r="C43" s="1"/>
+      <c r="D43" s="1"/>
+      <c r="E43" s="1">
+        <v>1</v>
+      </c>
+      <c r="F43" s="1"/>
+      <c r="G43" s="1"/>
+      <c r="H43" s="1"/>
+      <c r="I43" s="1"/>
+      <c r="J43" s="1"/>
+      <c r="K43" s="1"/>
+      <c r="L43" s="1"/>
+      <c r="M43" s="1"/>
+    </row>
+    <row r="44" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A44">
+        <v>25</v>
+      </c>
+      <c r="B44" s="1"/>
+      <c r="C44" s="1"/>
+      <c r="D44" s="1"/>
+      <c r="E44" s="1"/>
+      <c r="F44" s="1">
+        <v>1</v>
+      </c>
+      <c r="G44" s="1"/>
+      <c r="H44" s="1"/>
+      <c r="I44" s="1"/>
+      <c r="J44" s="1"/>
+      <c r="L44" s="1"/>
+    </row>
+    <row r="45" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A45">
+        <v>45</v>
+      </c>
+      <c r="B45" s="1"/>
+      <c r="C45" s="1"/>
+      <c r="D45" s="1"/>
+      <c r="E45" s="1"/>
+      <c r="F45" s="1"/>
+      <c r="G45" s="1">
+        <v>1</v>
+      </c>
+      <c r="I45" s="1"/>
+      <c r="K45" s="1"/>
+      <c r="L45" s="1"/>
+      <c r="M45" s="1"/>
+    </row>
+    <row r="46" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A46">
+        <v>13</v>
+      </c>
+      <c r="B46" s="1"/>
+      <c r="C46" s="1"/>
+      <c r="D46" s="1"/>
+      <c r="E46" s="1"/>
+      <c r="F46" s="1"/>
+      <c r="G46" s="1"/>
+      <c r="H46" s="1">
+        <v>1</v>
+      </c>
+      <c r="I46" s="1"/>
+      <c r="J46" s="1"/>
+      <c r="K46" s="1"/>
+      <c r="L46" s="1"/>
+      <c r="M46" s="1"/>
+    </row>
+    <row r="47" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A47">
+        <v>12</v>
+      </c>
+      <c r="B47" s="1"/>
+      <c r="C47" s="1"/>
+      <c r="D47" s="1"/>
+      <c r="E47" s="1"/>
+      <c r="F47" s="1"/>
+      <c r="G47" s="1"/>
+      <c r="H47" s="1"/>
+      <c r="I47" s="1">
+        <v>1</v>
+      </c>
+      <c r="J47" s="1"/>
+      <c r="K47" s="1"/>
+      <c r="L47" s="1"/>
+      <c r="M47" s="1"/>
+    </row>
+    <row r="53" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="B53" t="s">
+        <v>22</v>
+      </c>
+      <c r="J53" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="54" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A54" t="s">
+        <v>26</v>
+      </c>
+      <c r="B54">
+        <v>350</v>
+      </c>
+      <c r="C54">
+        <v>24</v>
+      </c>
+      <c r="D54">
+        <v>15</v>
+      </c>
+      <c r="E54">
+        <v>34</v>
+      </c>
+      <c r="F54">
+        <v>23</v>
+      </c>
+      <c r="G54">
+        <v>25</v>
+      </c>
+      <c r="H54">
+        <v>45</v>
+      </c>
+      <c r="I54">
+        <v>134</v>
+      </c>
+      <c r="J54">
+        <v>125</v>
+      </c>
+      <c r="K54">
+        <v>234</v>
+      </c>
+      <c r="L54">
+        <v>145</v>
+      </c>
+      <c r="M54">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="55" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A55" s="6">
+        <v>4</v>
+      </c>
+      <c r="B55" s="1"/>
+      <c r="C55" s="1"/>
+      <c r="D55" s="1"/>
+      <c r="E55" s="1"/>
+      <c r="F55" s="1"/>
+      <c r="G55" s="1"/>
+      <c r="H55" s="1"/>
+      <c r="I55" s="1"/>
+      <c r="K55" s="1"/>
+      <c r="L55" s="1"/>
+      <c r="M55" s="1"/>
+      <c r="N55" s="1"/>
+    </row>
+    <row r="56" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A56" s="6">
+        <v>5</v>
+      </c>
+      <c r="B56" s="1"/>
+      <c r="C56" s="1"/>
+      <c r="D56" s="1"/>
+      <c r="E56" s="1"/>
+      <c r="F56" s="1"/>
+      <c r="G56" s="1"/>
+      <c r="H56" s="1"/>
+      <c r="I56" s="1"/>
+      <c r="K56" s="1"/>
+      <c r="L56" s="1"/>
+      <c r="M56" s="1"/>
+      <c r="N56" s="1"/>
+    </row>
+    <row r="57" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A57" s="7">
+        <v>14</v>
+      </c>
+      <c r="B57" s="1"/>
+      <c r="C57" s="1"/>
+      <c r="D57" s="1"/>
+      <c r="E57" s="1"/>
+      <c r="F57" s="1"/>
+      <c r="G57" s="1"/>
+      <c r="H57" s="1"/>
+      <c r="I57" s="1"/>
+      <c r="K57" s="1"/>
+      <c r="L57" s="1"/>
+      <c r="M57" s="1"/>
+      <c r="N57" s="1"/>
+    </row>
+    <row r="58" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A58" s="7">
+        <v>35</v>
+      </c>
+      <c r="B58" s="1"/>
+      <c r="C58" s="1"/>
+      <c r="D58" s="1"/>
+      <c r="E58" s="1"/>
+      <c r="F58" s="1"/>
+      <c r="G58" s="1"/>
+      <c r="H58" s="1"/>
+      <c r="I58" s="1"/>
+      <c r="K58" s="1"/>
+      <c r="L58" s="1"/>
+      <c r="M58" s="1"/>
+      <c r="N58" s="1"/>
+    </row>
+    <row r="59" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A59">
+        <v>24</v>
+      </c>
+      <c r="B59" s="1"/>
+      <c r="C59" s="1"/>
+      <c r="D59" s="1"/>
+      <c r="E59" s="1"/>
+      <c r="F59" s="1"/>
+      <c r="G59" s="1"/>
+      <c r="H59" s="1"/>
+      <c r="I59" s="1"/>
+      <c r="K59" s="1"/>
+      <c r="L59" s="1"/>
+      <c r="M59" s="1"/>
+      <c r="N59" s="1"/>
+    </row>
+    <row r="60" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A60">
+        <v>15</v>
+      </c>
+      <c r="B60" s="1"/>
+      <c r="C60" s="1"/>
+      <c r="D60" s="1"/>
+      <c r="E60" s="1"/>
+      <c r="F60" s="1"/>
+      <c r="G60" s="1"/>
+      <c r="H60" s="1"/>
+      <c r="I60" s="1"/>
+      <c r="K60" s="1"/>
+      <c r="L60" s="1"/>
+      <c r="M60" s="1"/>
+      <c r="N60" s="1"/>
+    </row>
+    <row r="61" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A61">
+        <v>34</v>
+      </c>
+      <c r="B61" s="1"/>
+      <c r="C61" s="1"/>
+      <c r="D61" s="1"/>
+      <c r="E61" s="1"/>
+      <c r="F61" s="1"/>
+      <c r="G61" s="1"/>
+      <c r="H61" s="1"/>
+      <c r="I61" s="1"/>
+      <c r="K61" s="1"/>
+      <c r="L61" s="1"/>
+      <c r="M61" s="1"/>
+      <c r="N61" s="1"/>
+    </row>
+    <row r="62" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A62">
+        <v>23</v>
+      </c>
+      <c r="B62" s="1"/>
+      <c r="C62" s="1"/>
+      <c r="D62" s="1"/>
+      <c r="E62" s="1"/>
+      <c r="F62" s="1"/>
+      <c r="G62" s="1"/>
+      <c r="H62" s="1"/>
+      <c r="I62" s="1"/>
+      <c r="K62" s="1"/>
+      <c r="L62" s="1"/>
+      <c r="M62" s="1"/>
+      <c r="N62" s="1"/>
+    </row>
+    <row r="63" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A63">
+        <v>25</v>
+      </c>
+      <c r="B63" s="1"/>
+      <c r="C63" s="1"/>
+      <c r="D63" s="1"/>
+      <c r="E63" s="1"/>
+      <c r="F63" s="1"/>
+      <c r="G63" s="1"/>
+      <c r="H63" s="1"/>
+      <c r="I63" s="1"/>
+      <c r="K63" s="1"/>
+      <c r="M63" s="1"/>
+    </row>
+    <row r="64" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A64">
+        <v>45</v>
+      </c>
+      <c r="B64" s="1"/>
+      <c r="C64" s="1"/>
+      <c r="D64" s="1"/>
+      <c r="E64" s="1"/>
+      <c r="F64" s="1"/>
+      <c r="G64" s="1"/>
+      <c r="I64" s="1"/>
+      <c r="L64" s="1"/>
+      <c r="M64" s="1"/>
+      <c r="N64" s="1"/>
+    </row>
+    <row r="65" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A65">
+        <v>13</v>
+      </c>
+      <c r="B65" s="1"/>
+      <c r="C65" s="1"/>
+      <c r="D65" s="1"/>
+      <c r="E65" s="1"/>
+      <c r="F65" s="1"/>
+      <c r="G65" s="1"/>
+      <c r="H65" s="1"/>
+      <c r="I65" s="1"/>
+      <c r="K65" s="1"/>
+      <c r="L65" s="1"/>
+      <c r="M65" s="1"/>
+      <c r="N65" s="1"/>
+    </row>
+    <row r="66" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A66">
+        <v>12</v>
+      </c>
+      <c r="B66" s="1"/>
+      <c r="C66" s="1"/>
+      <c r="D66" s="1"/>
+      <c r="E66" s="1"/>
+      <c r="F66" s="1"/>
+      <c r="G66" s="1"/>
+      <c r="H66" s="1"/>
+      <c r="I66" s="1"/>
+      <c r="K66" s="1"/>
+      <c r="L66" s="1"/>
+      <c r="M66" s="1"/>
+      <c r="N66" s="1"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U15"/>
   <sheetViews>
@@ -4211,729 +6401,4 @@
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M14"/>
-  <sheetViews>
-    <sheetView zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
-      <selection activeCell="O15" sqref="O15"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="8" width="3.5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="3.5" customWidth="1"/>
-    <col min="10" max="14" width="4.5" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>26</v>
-      </c>
-      <c r="B1">
-        <v>35</v>
-      </c>
-      <c r="C1">
-        <v>14</v>
-      </c>
-      <c r="D1">
-        <v>24</v>
-      </c>
-      <c r="E1">
-        <v>15</v>
-      </c>
-      <c r="F1">
-        <v>34</v>
-      </c>
-      <c r="G1">
-        <v>25</v>
-      </c>
-      <c r="H1">
-        <v>13</v>
-      </c>
-      <c r="I1">
-        <v>45</v>
-      </c>
-      <c r="J1">
-        <v>125</v>
-      </c>
-      <c r="K1">
-        <v>234</v>
-      </c>
-      <c r="L1">
-        <v>124</v>
-      </c>
-      <c r="M1">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A2" s="6">
-        <v>4</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
-      <c r="G2" s="1"/>
-      <c r="H2" s="1"/>
-      <c r="I2" s="1"/>
-      <c r="J2" s="1"/>
-      <c r="K2" s="1">
-        <v>-1</v>
-      </c>
-      <c r="L2" s="1">
-        <v>-1</v>
-      </c>
-      <c r="M2" s="1"/>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A3" s="6">
-        <v>5</v>
-      </c>
-      <c r="B3" s="1"/>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
-      <c r="G3" s="1"/>
-      <c r="H3" s="1"/>
-      <c r="I3" s="1"/>
-      <c r="J3" s="1">
-        <v>-1</v>
-      </c>
-      <c r="K3" s="1"/>
-      <c r="L3" s="1"/>
-      <c r="M3" s="1">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A4">
-        <v>35</v>
-      </c>
-      <c r="B4" s="1">
-        <v>1</v>
-      </c>
-      <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
-      <c r="E4" s="1"/>
-      <c r="F4" s="1"/>
-      <c r="G4" s="1"/>
-      <c r="H4" s="1"/>
-      <c r="I4" s="1"/>
-      <c r="J4" s="1"/>
-      <c r="K4" s="1"/>
-      <c r="L4" s="1"/>
-      <c r="M4" s="1">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A5">
-        <v>14</v>
-      </c>
-      <c r="B5" s="1"/>
-      <c r="C5" s="1">
-        <v>1</v>
-      </c>
-      <c r="D5" s="1"/>
-      <c r="E5" s="1"/>
-      <c r="F5" s="1"/>
-      <c r="G5" s="1"/>
-      <c r="H5" s="1"/>
-      <c r="I5" s="1"/>
-      <c r="J5" s="1"/>
-      <c r="K5" s="1"/>
-      <c r="L5" s="1">
-        <v>-1</v>
-      </c>
-      <c r="M5" s="1"/>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A6">
-        <v>24</v>
-      </c>
-      <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1">
-        <v>1</v>
-      </c>
-      <c r="E6" s="1"/>
-      <c r="F6" s="1"/>
-      <c r="G6" s="1"/>
-      <c r="H6" s="1"/>
-      <c r="I6" s="1"/>
-      <c r="J6" s="1"/>
-      <c r="K6" s="1">
-        <v>-1</v>
-      </c>
-      <c r="L6" s="1">
-        <v>-1</v>
-      </c>
-      <c r="M6" s="1"/>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A7">
-        <v>15</v>
-      </c>
-      <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
-      <c r="D7" s="1"/>
-      <c r="E7" s="1">
-        <v>1</v>
-      </c>
-      <c r="F7" s="1"/>
-      <c r="G7" s="1"/>
-      <c r="H7" s="1"/>
-      <c r="I7" s="1"/>
-      <c r="J7" s="1">
-        <v>-1</v>
-      </c>
-      <c r="K7" s="1"/>
-      <c r="L7" s="1"/>
-      <c r="M7" s="1">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A8">
-        <v>34</v>
-      </c>
-      <c r="B8" s="1"/>
-      <c r="C8" s="1"/>
-      <c r="D8" s="1"/>
-      <c r="E8" s="1"/>
-      <c r="F8" s="1">
-        <v>1</v>
-      </c>
-      <c r="G8" s="1"/>
-      <c r="H8" s="1"/>
-      <c r="I8" s="1"/>
-      <c r="J8" s="1"/>
-      <c r="K8" s="1">
-        <v>-1</v>
-      </c>
-      <c r="L8" s="1"/>
-      <c r="M8" s="1"/>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A9">
-        <v>25</v>
-      </c>
-      <c r="B9" s="1"/>
-      <c r="C9" s="1"/>
-      <c r="D9" s="1"/>
-      <c r="E9" s="1"/>
-      <c r="F9" s="1"/>
-      <c r="G9" s="1">
-        <v>1</v>
-      </c>
-      <c r="H9" s="1"/>
-      <c r="I9" s="1"/>
-      <c r="J9" s="1">
-        <v>-1</v>
-      </c>
-      <c r="K9" s="1"/>
-      <c r="L9" s="1"/>
-      <c r="M9" s="1"/>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A10">
-        <v>13</v>
-      </c>
-      <c r="B10" s="1"/>
-      <c r="C10" s="1"/>
-      <c r="D10" s="1"/>
-      <c r="E10" s="1"/>
-      <c r="F10" s="1"/>
-      <c r="G10" s="1"/>
-      <c r="H10" s="1">
-        <v>1</v>
-      </c>
-      <c r="I10" s="1"/>
-      <c r="J10" s="1"/>
-      <c r="K10" s="1"/>
-      <c r="L10" s="1"/>
-      <c r="M10" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A11">
-        <v>45</v>
-      </c>
-      <c r="B11" s="1"/>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
-      <c r="E11" s="1"/>
-      <c r="F11" s="1"/>
-      <c r="G11" s="1"/>
-      <c r="H11" s="1"/>
-      <c r="I11" s="1">
-        <v>1</v>
-      </c>
-      <c r="J11" s="1"/>
-      <c r="K11" s="1"/>
-      <c r="L11" s="1"/>
-      <c r="M11" s="1"/>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A12" s="7">
-        <v>12</v>
-      </c>
-      <c r="B12" s="1"/>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
-      <c r="E12" s="1"/>
-      <c r="F12" s="1"/>
-      <c r="G12" s="1"/>
-      <c r="H12" s="1"/>
-      <c r="I12" s="1"/>
-      <c r="J12" s="1">
-        <v>1</v>
-      </c>
-      <c r="K12" s="1"/>
-      <c r="L12" s="1">
-        <v>1</v>
-      </c>
-      <c r="M12" s="1"/>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A13" s="6">
-        <v>23</v>
-      </c>
-      <c r="B13" s="1"/>
-      <c r="C13" s="1"/>
-      <c r="D13" s="1"/>
-      <c r="E13" s="1"/>
-      <c r="F13" s="1"/>
-      <c r="G13" s="1"/>
-      <c r="H13" s="1"/>
-      <c r="I13" s="1"/>
-      <c r="J13" s="1"/>
-      <c r="K13" s="1">
-        <v>1</v>
-      </c>
-      <c r="L13" s="1"/>
-      <c r="M13" s="1"/>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="K14" s="5"/>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G27"/>
-  <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="J32" sqref="J32"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
-  <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A1">
-        <v>4</v>
-      </c>
-      <c r="C1">
-        <v>4</v>
-      </c>
-      <c r="E1">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A2">
-        <v>5</v>
-      </c>
-      <c r="C2">
-        <v>5</v>
-      </c>
-      <c r="E2">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>31</v>
-      </c>
-      <c r="B3" t="s">
-        <v>32</v>
-      </c>
-      <c r="C3" t="str">
-        <f>_xlfn.CONCAT(A3,B3)</f>
-        <v xml:space="preserve"> (1 2)</v>
-      </c>
-      <c r="E3" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>31</v>
-      </c>
-      <c r="B4" t="s">
-        <v>33</v>
-      </c>
-      <c r="C4" t="str">
-        <f t="shared" ref="C4:C12" si="0">_xlfn.CONCAT(A4,B4)</f>
-        <v xml:space="preserve"> (1 3)</v>
-      </c>
-      <c r="E4" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>34</v>
-      </c>
-      <c r="B5" t="s">
-        <v>33</v>
-      </c>
-      <c r="C5" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve"> (2 3)</v>
-      </c>
-      <c r="E5" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>31</v>
-      </c>
-      <c r="B6" t="s">
-        <v>35</v>
-      </c>
-      <c r="C6" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve"> (1 4)</v>
-      </c>
-      <c r="E6" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>34</v>
-      </c>
-      <c r="B7" t="s">
-        <v>35</v>
-      </c>
-      <c r="C7" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve"> (2 4)</v>
-      </c>
-      <c r="E7" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>36</v>
-      </c>
-      <c r="B8" t="s">
-        <v>35</v>
-      </c>
-      <c r="C8" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve"> (3 4)</v>
-      </c>
-      <c r="E8" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>31</v>
-      </c>
-      <c r="B9" t="s">
-        <v>37</v>
-      </c>
-      <c r="C9" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve"> (1 5)</v>
-      </c>
-      <c r="E9" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>34</v>
-      </c>
-      <c r="B10" t="s">
-        <v>37</v>
-      </c>
-      <c r="C10" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve"> (2 5)</v>
-      </c>
-      <c r="E10" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>36</v>
-      </c>
-      <c r="B11" t="s">
-        <v>37</v>
-      </c>
-      <c r="C11" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve"> (3 5)</v>
-      </c>
-      <c r="E11" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>38</v>
-      </c>
-      <c r="B12" t="s">
-        <v>37</v>
-      </c>
-      <c r="C12" t="str">
-        <f t="shared" si="0"/>
-        <v xml:space="preserve"> (4 5)</v>
-      </c>
-      <c r="E12" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
-        <v>49</v>
-      </c>
-      <c r="B16" t="s">
-        <v>37</v>
-      </c>
-      <c r="C16" t="s">
-        <v>50</v>
-      </c>
-      <c r="E16" t="str">
-        <f>_xlfn.CONCAT(A16,B16,C16)</f>
-        <v>((3 5) None)</v>
-      </c>
-      <c r="G16" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
-        <v>51</v>
-      </c>
-      <c r="B17" t="s">
-        <v>35</v>
-      </c>
-      <c r="C17" t="s">
-        <v>50</v>
-      </c>
-      <c r="E17" t="str">
-        <f t="shared" ref="E17:E27" si="1">_xlfn.CONCAT(A17,B17,C17)</f>
-        <v xml:space="preserve"> ((2 4) None)</v>
-      </c>
-      <c r="G17" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
-        <v>52</v>
-      </c>
-      <c r="B18" t="s">
-        <v>35</v>
-      </c>
-      <c r="C18" t="s">
-        <v>37</v>
-      </c>
-      <c r="E18" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve"> ((1 4) 5)</v>
-      </c>
-      <c r="G18" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
-        <v>52</v>
-      </c>
-      <c r="B19" t="s">
-        <v>37</v>
-      </c>
-      <c r="C19" t="s">
-        <v>50</v>
-      </c>
-      <c r="E19" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve"> ((1 5) None)</v>
-      </c>
-      <c r="G19" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
-        <v>53</v>
-      </c>
-      <c r="B20" t="s">
-        <v>35</v>
-      </c>
-      <c r="C20" t="s">
-        <v>50</v>
-      </c>
-      <c r="E20" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve"> ((3 4) None)</v>
-      </c>
-      <c r="G20" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
-        <v>51</v>
-      </c>
-      <c r="B21" t="s">
-        <v>37</v>
-      </c>
-      <c r="C21" t="s">
-        <v>50</v>
-      </c>
-      <c r="E21" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve"> ((2 5) None)</v>
-      </c>
-      <c r="G21" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
-        <v>52</v>
-      </c>
-      <c r="B22" t="s">
-        <v>33</v>
-      </c>
-      <c r="C22" t="s">
-        <v>50</v>
-      </c>
-      <c r="E22" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve"> ((1 3) None)</v>
-      </c>
-      <c r="G22" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A23" t="s">
-        <v>54</v>
-      </c>
-      <c r="B23" t="s">
-        <v>37</v>
-      </c>
-      <c r="C23" t="s">
-        <v>50</v>
-      </c>
-      <c r="E23" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve"> ((4 5) None)</v>
-      </c>
-      <c r="G23" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A24" t="s">
-        <v>51</v>
-      </c>
-      <c r="B24" t="s">
-        <v>33</v>
-      </c>
-      <c r="C24" t="s">
-        <v>35</v>
-      </c>
-      <c r="E24" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve"> ((2 3) 4)</v>
-      </c>
-      <c r="G24" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A25" t="s">
-        <v>52</v>
-      </c>
-      <c r="B25" t="s">
-        <v>32</v>
-      </c>
-      <c r="C25" t="s">
-        <v>50</v>
-      </c>
-      <c r="E25" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve"> ((1 2) None)</v>
-      </c>
-      <c r="G25" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A26" t="s">
-        <v>52</v>
-      </c>
-      <c r="B26" t="s">
-        <v>33</v>
-      </c>
-      <c r="C26" t="s">
-        <v>35</v>
-      </c>
-      <c r="E26" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve"> ((1 3) 4)</v>
-      </c>
-      <c r="G26" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A27" t="s">
-        <v>52</v>
-      </c>
-      <c r="B27" t="s">
-        <v>33</v>
-      </c>
-      <c r="C27" t="s">
-        <v>37</v>
-      </c>
-      <c r="E27" t="str">
-        <f t="shared" si="1"/>
-        <v xml:space="preserve"> ((1 3) 5)</v>
-      </c>
-      <c r="G27" t="s">
-        <v>66</v>
-      </c>
-    </row>
-  </sheetData>
-  <dataConsolidate/>
-  <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>